<commit_message>
add functionality and documentation
</commit_message>
<xml_diff>
--- a/additional_info/data_dictionary.xlsx
+++ b/additional_info/data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fakhriakmalh/Documents/CV_updated/fithub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fakhriakmalh/Documents/CV_updated/fithub/projects/additional_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC04BD4C-61C7-5742-9E98-13DD1C33343F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E968286E-B36D-B24C-9D0C-5C6C2FDF387E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{1BD56C6F-1B0D-B640-81C6-24C79F60B4CB}"/>
   </bookViews>
@@ -167,12 +167,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>unique log id</t>
-  </si>
-  <si>
-    <t>Unique identifier for the referral.</t>
-  </si>
-  <si>
     <t>Source of the referral (e.g., "User Sign Up", "Draft Transaction","Lead")</t>
   </si>
   <si>
@@ -251,12 +245,18 @@
       <t>logic in questions</t>
     </r>
   </si>
+  <si>
+    <t>Unique identifier for the referral</t>
+  </si>
+  <si>
+    <t>Unique log id of the referral</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +285,13 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -348,7 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -356,6 +362,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +700,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -734,8 +741,8 @@
       <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>43</v>
+      <c r="E2" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -751,11 +758,11 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="64">
+      <c r="E3" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -768,8 +775,8 @@
       <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>45</v>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32">
@@ -783,10 +790,10 @@
         <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>66</v>
+        <v>44</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -802,8 +809,8 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>47</v>
+      <c r="E6" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -819,8 +826,8 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>48</v>
+      <c r="E7" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -834,10 +841,10 @@
         <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -853,8 +860,8 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>50</v>
+      <c r="E9" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -870,8 +877,8 @@
       <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>52</v>
+      <c r="E10" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -887,8 +894,8 @@
       <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>53</v>
+      <c r="E11" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -904,8 +911,8 @@
       <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>54</v>
+      <c r="E12" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -921,8 +928,8 @@
       <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>55</v>
+      <c r="E13" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -938,8 +945,8 @@
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>56</v>
+      <c r="E14" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -955,8 +962,8 @@
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>57</v>
+      <c r="E15" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -972,8 +979,8 @@
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>58</v>
+      <c r="E16" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -989,8 +996,8 @@
       <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>59</v>
+      <c r="E17" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1006,8 +1013,8 @@
       <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>60</v>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1023,8 +1030,8 @@
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>61</v>
+      <c r="E19" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1040,8 +1047,8 @@
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>62</v>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1057,8 +1064,8 @@
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>63</v>
+      <c r="E21" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1074,8 +1081,8 @@
       <c r="D22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>65</v>
+      <c r="E22" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1089,8 +1096,8 @@
         <v>41</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="8" t="s">
-        <v>64</v>
+      <c r="E23" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>